<commit_message>
Removed cc to support email
</commit_message>
<xml_diff>
--- a/public/sample_uploads/capital_calls.xlsx
+++ b/public/sample_uploads/capital_calls.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thimm\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\thimmaiah\work\IRM\public\sample_uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{192A3579-CF46-421B-8E0C-E45C44D8B93A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3545BB95-731D-4A23-8F64-DE73AE26B515}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,18 +22,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
-    <t>Fund</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Percentage Called</t>
-  </si>
-  <si>
-    <t>Due Date</t>
-  </si>
-  <si>
     <t>Agri Fund</t>
   </si>
   <si>
@@ -44,6 +32,18 @@
   </si>
   <si>
     <t>Capital Call 6</t>
+  </si>
+  <si>
+    <t>Fund *</t>
+  </si>
+  <si>
+    <t>Name *</t>
+  </si>
+  <si>
+    <t>Percentage Called *</t>
+  </si>
+  <si>
+    <t>Due Date *</t>
   </si>
 </sst>
 </file>
@@ -397,7 +397,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.35"/>
@@ -410,24 +410,24 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C2">
         <v>30</v>
@@ -438,10 +438,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C3">
         <v>10</v>
@@ -452,10 +452,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C4">
         <v>30</v>

</xml_diff>

<commit_message>
Added better support for importing capital calls & distributions
</commit_message>
<xml_diff>
--- a/public/sample_uploads/capital_calls.xlsx
+++ b/public/sample_uploads/capital_calls.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\thimmaiah\work\IRM\public\sample_uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3545BB95-731D-4A23-8F64-DE73AE26B515}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD6D2BBE-80CC-402D-9147-5A2EE1BADF7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
   <si>
     <t>Agri Fund</t>
   </si>
@@ -44,6 +44,18 @@
   </si>
   <si>
     <t>Due Date *</t>
+  </si>
+  <si>
+    <t>Generate Remittances</t>
+  </si>
+  <si>
+    <t>Remittances Verified</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -394,10 +406,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.35"/>
@@ -406,9 +418,11 @@
     <col min="2" max="2" width="18.6875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.3125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.0625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.6875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -421,8 +435,14 @@
       <c r="D1" t="s">
         <v>7</v>
       </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -435,8 +455,14 @@
       <c r="D2" s="1">
         <v>44914</v>
       </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -449,8 +475,14 @@
       <c r="D3" s="1">
         <v>44914</v>
       </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -462,6 +494,12 @@
       </c>
       <c r="D4" s="1">
         <v>44914</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added tests for fund uploads
</commit_message>
<xml_diff>
--- a/public/sample_uploads/capital_calls.xlsx
+++ b/public/sample_uploads/capital_calls.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\thimmaiah\work\IRM\public\sample_uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD6D2BBE-80CC-402D-9147-5A2EE1BADF7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDA175D6-29BA-47B0-B934-9B27022CA4C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,9 +22,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
   <si>
-    <t>Agri Fund</t>
-  </si>
-  <si>
     <t>Capital Call 4</t>
   </si>
   <si>
@@ -56,6 +53,9 @@
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>SAAS Fund</t>
   </si>
 </sst>
 </file>
@@ -409,7 +409,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.35"/>
@@ -424,30 +424,30 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>8</v>
-      </c>
-      <c r="F1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
         <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
       </c>
       <c r="C2">
         <v>30</v>
@@ -456,18 +456,18 @@
         <v>44914</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3">
         <v>10</v>
@@ -476,18 +476,18 @@
         <v>44914</v>
       </c>
       <c r="E3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" t="s">
         <v>10</v>
-      </c>
-      <c r="F3" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4">
         <v>30</v>
@@ -496,10 +496,10 @@
         <v>44914</v>
       </c>
       <c r="E4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added bulk import of distribution payments
</commit_message>
<xml_diff>
--- a/public/sample_uploads/capital_calls.xlsx
+++ b/public/sample_uploads/capital_calls.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\thimmaiah\work\IRM\public\sample_uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDA175D6-29BA-47B0-B934-9B27022CA4C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7C3D745-3E61-47A8-A9D4-B253C3E14425}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -409,7 +409,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.35"/>
@@ -496,7 +496,7 @@
         <v>44914</v>
       </c>
       <c r="E4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F4" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
Added minor fixes to FX, still not fixed fully
</commit_message>
<xml_diff>
--- a/public/sample_uploads/capital_calls.xlsx
+++ b/public/sample_uploads/capital_calls.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\thimmaiah\work\IRM\public\sample_uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A3A08D2-AE36-438D-8777-A1FC616ACA88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77CAC4AF-ED38-4425-912A-7CD92017E2B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="24">
   <si>
     <t>Fund *</t>
   </si>
@@ -79,6 +79,24 @@
   </si>
   <si>
     <t>CoInvest</t>
+  </si>
+  <si>
+    <t>From Currency</t>
+  </si>
+  <si>
+    <t>To Currency</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exchange Rate </t>
+  </si>
+  <si>
+    <t>As Of</t>
+  </si>
+  <si>
+    <t>USD</t>
+  </si>
+  <si>
+    <t>INR</t>
   </si>
 </sst>
 </file>
@@ -434,10 +452,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView tabSelected="1" showOutlineSymbols="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="13.5" x14ac:dyDescent="0.35"/>
@@ -448,9 +466,10 @@
     <col min="5" max="6" width="14.3125" customWidth="1"/>
     <col min="7" max="7" width="19.0625" customWidth="1"/>
     <col min="8" max="8" width="17.6875" customWidth="1"/>
+    <col min="13" max="13" width="9.9375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -478,8 +497,20 @@
       <c r="I1" t="s">
         <v>13</v>
       </c>
+      <c r="J1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M1" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -493,10 +524,10 @@
         <v>30</v>
       </c>
       <c r="E2" s="1">
-        <v>44905</v>
+        <v>44571</v>
       </c>
       <c r="F2" s="2">
-        <v>44914</v>
+        <v>44580</v>
       </c>
       <c r="G2" t="s">
         <v>9</v>
@@ -507,8 +538,20 @@
       <c r="I2" t="s">
         <v>14</v>
       </c>
+      <c r="J2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L2">
+        <v>80</v>
+      </c>
+      <c r="M2" s="1">
+        <v>44571</v>
+      </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -522,10 +565,10 @@
         <v>10</v>
       </c>
       <c r="E3" s="1">
-        <v>44905</v>
+        <v>44722</v>
       </c>
       <c r="F3" s="2">
-        <v>44914</v>
+        <v>44731</v>
       </c>
       <c r="G3" t="s">
         <v>9</v>
@@ -536,8 +579,20 @@
       <c r="I3" t="s">
         <v>14</v>
       </c>
+      <c r="J3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" t="s">
+        <v>23</v>
+      </c>
+      <c r="L3">
+        <v>81</v>
+      </c>
+      <c r="M3" s="1">
+        <v>44722</v>
+      </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -564,6 +619,18 @@
       </c>
       <c r="I4" t="s">
         <v>14</v>
+      </c>
+      <c r="J4" t="s">
+        <v>22</v>
+      </c>
+      <c r="K4" t="s">
+        <v>23</v>
+      </c>
+      <c r="L4">
+        <v>82</v>
+      </c>
+      <c r="M4" s="1">
+        <v>44905</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added exchange rates sheet for capital calls upload
</commit_message>
<xml_diff>
--- a/public/sample_uploads/capital_calls.xlsx
+++ b/public/sample_uploads/capital_calls.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\thimmaiah\work\IRM\public\sample_uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77CAC4AF-ED38-4425-912A-7CD92017E2B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22672C02-1B34-41E2-B8E0-F899AAA906B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CapitalCall" sheetId="1" r:id="rId1"/>
+    <sheet name="Exchange Rates" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -452,10 +453,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" showOutlineSymbols="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="13.5" x14ac:dyDescent="0.35"/>
@@ -469,7 +470,7 @@
     <col min="13" max="13" width="9.9375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -497,20 +498,8 @@
       <c r="I1" t="s">
         <v>13</v>
       </c>
-      <c r="J1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K1" t="s">
-        <v>19</v>
-      </c>
-      <c r="L1" t="s">
-        <v>20</v>
-      </c>
-      <c r="M1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -538,20 +527,8 @@
       <c r="I2" t="s">
         <v>14</v>
       </c>
-      <c r="J2" t="s">
-        <v>22</v>
-      </c>
-      <c r="K2" t="s">
-        <v>23</v>
-      </c>
-      <c r="L2">
-        <v>80</v>
-      </c>
-      <c r="M2" s="1">
-        <v>44571</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -579,20 +556,8 @@
       <c r="I3" t="s">
         <v>14</v>
       </c>
-      <c r="J3" t="s">
-        <v>22</v>
-      </c>
-      <c r="K3" t="s">
-        <v>23</v>
-      </c>
-      <c r="L3">
-        <v>81</v>
-      </c>
-      <c r="M3" s="1">
-        <v>44722</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -619,22 +584,81 @@
       </c>
       <c r="I4" t="s">
         <v>14</v>
-      </c>
-      <c r="J4" t="s">
-        <v>22</v>
-      </c>
-      <c r="K4" t="s">
-        <v>23</v>
-      </c>
-      <c r="L4">
-        <v>82</v>
-      </c>
-      <c r="M4" s="1">
-        <v>44905</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1B98F01-16E8-4971-9FC7-B6A084ED76B8}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2">
+        <v>80</v>
+      </c>
+      <c r="D2" s="1">
+        <v>44571</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3">
+        <v>81</v>
+      </c>
+      <c r="D3" s="1">
+        <v>44722</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4">
+        <v>82</v>
+      </c>
+      <c r="D4" s="1">
+        <v>44905</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed bug with remittance payment date being nil
</commit_message>
<xml_diff>
--- a/public/sample_uploads/capital_calls.xlsx
+++ b/public/sample_uploads/capital_calls.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\thimmaiah\work\IRM\public\sample_uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D756A28E-A146-44AE-995D-A7921A21AC40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8753C7F-E87A-4719-A3B4-525F0DD7D04D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -462,7 +462,7 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" showOutlineSymbols="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="13.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Added import of unit_prices in calls
</commit_message>
<xml_diff>
--- a/public/sample_uploads/capital_calls.xlsx
+++ b/public/sample_uploads/capital_calls.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\thimmaiah\work\IRM\public\sample_uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FF63C15-0A83-4A17-B386-274FE5D7E3C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCDD48ED-5FFC-4503-8187-34366E76FDB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -286,7 +286,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{0B4F53B0-A7E9-47F4-8639-5EFB7FF6D084}">
+    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{0B4F53B0-A7E9-47F4-8639-5EFB7FF6D084}">
       <text>
         <r>
           <rPr>
@@ -435,7 +435,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="29">
   <si>
     <t>Fund *</t>
   </si>
@@ -513,6 +513,15 @@
   </si>
   <si>
     <t>Percentage of Commitment</t>
+  </si>
+  <si>
+    <t>Unit Price/Premium</t>
+  </si>
+  <si>
+    <t>Series A:100:0,Series B:110:10,Series C:120:20</t>
+  </si>
+  <si>
+    <t>Series A:1000:0,Series B:1100:100,Series C:1200:200</t>
   </si>
 </sst>
 </file>
@@ -919,10 +928,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView tabSelected="1" showOutlineSymbols="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -937,12 +946,13 @@
     <col min="8" max="8" width="17.875" style="3" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.0625" style="3" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="21.4375" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="8.625" style="3"/>
-    <col min="13" max="13" width="10" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.625" style="3"/>
+    <col min="11" max="11" width="21.4375" style="3" customWidth="1"/>
+    <col min="12" max="13" width="8.625" style="3"/>
+    <col min="14" max="14" width="10" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="8.625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -973,9 +983,12 @@
       <c r="J1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="K1" s="2"/>
+      <c r="K1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L1" s="2"/>
     </row>
-    <row r="2" spans="1:11" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
@@ -1006,8 +1019,11 @@
       <c r="J2" s="3" t="s">
         <v>25</v>
       </c>
+      <c r="K2" s="3" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="3" spans="1:11" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
@@ -1038,8 +1054,11 @@
       <c r="J3" s="3" t="s">
         <v>25</v>
       </c>
+      <c r="K3" s="3" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="4" spans="1:11" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
@@ -1070,8 +1089,11 @@
       <c r="J4" s="3" t="s">
         <v>25</v>
       </c>
+      <c r="K4" s="3" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="6" spans="1:11" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A6"/>
       <c r="C6"/>
       <c r="D6"/>
@@ -1079,7 +1101,7 @@
       <c r="F6"/>
       <c r="I6"/>
     </row>
-    <row r="7" spans="1:11" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A7"/>
       <c r="C7"/>
       <c r="D7"/>
@@ -1087,7 +1109,7 @@
       <c r="F7"/>
       <c r="I7"/>
     </row>
-    <row r="8" spans="1:11" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A8"/>
       <c r="C8"/>
       <c r="D8"/>
@@ -1095,7 +1117,7 @@
       <c r="F8"/>
       <c r="I8"/>
     </row>
-    <row r="9" spans="1:11" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A9"/>
       <c r="C9"/>
       <c r="D9"/>
@@ -1111,7 +1133,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:H1048576" xr:uid="{11B9AB33-F501-46FE-9E66-0C8FF70AF92A}">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J1048576" xr:uid="{D03DE4C3-CD9D-4566-9C86-F32A60B115D9}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J1048576 K6:K1048576" xr:uid="{D03DE4C3-CD9D-4566-9C86-F32A60B115D9}">
       <formula1>"Percentage of Commitment,Upload"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Lazy load access rights (#368)
* Added send_notification_flag to call

* Added CapitalRemittancePaymentMailer

* Added payment_notification_sent to remittance payment to avoid dups

* Added payment_notification_sent to remittance payment to avoid dups

* Hide fields in remittance show which are not filled

* Improved custom notifications for payment

* Changed label for notifications label

* Now lazy loads access_rights in multiple places
</commit_message>
<xml_diff>
--- a/public/sample_uploads/capital_calls.xlsx
+++ b/public/sample_uploads/capital_calls.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\thimmaiah\work\IRM\public\sample_uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCDD48ED-5FFC-4503-8187-34366E76FDB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FB4C226-D3D8-41D8-9E60-F67C4C55A04E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15" yWindow="735" windowWidth="23985" windowHeight="14265" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CapitalCall" sheetId="1" r:id="rId1"/>
@@ -286,7 +286,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{0B4F53B0-A7E9-47F4-8639-5EFB7FF6D084}">
+    <comment ref="N1" authorId="0" shapeId="0" xr:uid="{0B4F53B0-A7E9-47F4-8639-5EFB7FF6D084}">
       <text>
         <r>
           <rPr>
@@ -435,7 +435,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="31">
   <si>
     <t>Fund *</t>
   </si>
@@ -522,6 +522,12 @@
   </si>
   <si>
     <t>Series A:1000:0,Series B:1100:100,Series C:1200:200</t>
+  </si>
+  <si>
+    <t>Send Call Notice</t>
+  </si>
+  <si>
+    <t>Send Payment Notification</t>
   </si>
 </sst>
 </file>
@@ -928,10 +934,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView tabSelected="1" showOutlineSymbols="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -946,13 +952,13 @@
     <col min="8" max="8" width="17.875" style="3" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.0625" style="3" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="21.4375" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.4375" style="3" customWidth="1"/>
-    <col min="12" max="13" width="8.625" style="3"/>
-    <col min="14" max="14" width="10" style="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="8.625" style="3"/>
+    <col min="11" max="13" width="21.4375" style="3" customWidth="1"/>
+    <col min="14" max="15" width="8.625" style="3"/>
+    <col min="16" max="16" width="10" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="8.625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -986,9 +992,15 @@
       <c r="K1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="L1" s="2"/>
+      <c r="L1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="N1" s="2"/>
     </row>
-    <row r="2" spans="1:12" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
@@ -1022,8 +1034,14 @@
       <c r="K2" s="3" t="s">
         <v>27</v>
       </c>
+      <c r="L2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="3" spans="1:12" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
@@ -1057,8 +1075,14 @@
       <c r="K3" s="3" t="s">
         <v>27</v>
       </c>
+      <c r="L3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="4" spans="1:12" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
@@ -1092,8 +1116,14 @@
       <c r="K4" s="3" t="s">
         <v>28</v>
       </c>
+      <c r="L4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="6" spans="1:12" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A6"/>
       <c r="C6"/>
       <c r="D6"/>
@@ -1101,7 +1131,7 @@
       <c r="F6"/>
       <c r="I6"/>
     </row>
-    <row r="7" spans="1:12" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A7"/>
       <c r="C7"/>
       <c r="D7"/>
@@ -1109,7 +1139,7 @@
       <c r="F7"/>
       <c r="I7"/>
     </row>
-    <row r="8" spans="1:12" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A8"/>
       <c r="C8"/>
       <c r="D8"/>
@@ -1117,7 +1147,7 @@
       <c r="F8"/>
       <c r="I8"/>
     </row>
-    <row r="9" spans="1:12" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A9"/>
       <c r="C9"/>
       <c r="D9"/>
@@ -1133,7 +1163,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:H1048576" xr:uid="{11B9AB33-F501-46FE-9E66-0C8FF70AF92A}">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J1048576 K6:K1048576" xr:uid="{D03DE4C3-CD9D-4566-9C86-F32A60B115D9}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J1048576 K6:M1048576" xr:uid="{D03DE4C3-CD9D-4566-9C86-F32A60B115D9}">
       <formula1>"Percentage of Commitment,Upload"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Import cc fixes (#465)
* Import capital call for close percentages

* Validation for Upload call basis

* Specs for uploads

* Specs for uploads

* Specs for uploads
</commit_message>
<xml_diff>
--- a/public/sample_uploads/capital_calls.xlsx
+++ b/public/sample_uploads/capital_calls.xlsx
@@ -262,30 +262,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Author:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">-Incase custom fields are already created, please download the data from the platform to use existing headers to avoid errors while generating documents
--Can add any custom fields as per your requirement</t>
-        </r>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
@@ -397,7 +373,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="34">
   <si>
     <t xml:space="preserve">Fund *</t>
   </si>
@@ -438,9 +414,6 @@
     <t xml:space="preserve">Send Call Notice</t>
   </si>
   <si>
-    <t xml:space="preserve">Close Percentages</t>
-  </si>
-  <si>
     <t xml:space="preserve">SAAS Fund</t>
   </si>
   <si>
@@ -462,18 +435,12 @@
     <t xml:space="preserve">Series A:100:0,Series B:110:10,Series C:120:20</t>
   </si>
   <si>
-    <t xml:space="preserve">{“First Close”: “30”}</t>
-  </si>
-  <si>
     <t xml:space="preserve">Capital Call 8</t>
   </si>
   <si>
     <t xml:space="preserve">No</t>
   </si>
   <si>
-    <t xml:space="preserve">{“First Close”: “10”}</t>
-  </si>
-  <si>
     <t xml:space="preserve">CoInvest</t>
   </si>
   <si>
@@ -481,6 +448,15 @@
   </si>
   <si>
     <t xml:space="preserve">Series A:1000:0,Series B:1100:100,Series C:1200:200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Capital Call 9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30, 10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">First Close, Second Close</t>
   </si>
   <si>
     <t xml:space="preserve">From Currency</t>
@@ -614,32 +590,24 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -834,8 +802,8 @@
   </sheetPr>
   <dimension ref="A1:N9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N7" activeCellId="0" sqref="N7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N5" activeCellId="0" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -855,7 +823,7 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="17" style="1" width="8.62"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -895,151 +863,181 @@
       <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="3" t="s">
-        <v>13</v>
-      </c>
+      <c r="N1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="D2" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="E2" s="4" t="n">
+      <c r="E2" s="3" t="n">
         <v>44571</v>
       </c>
-      <c r="F2" s="5" t="n">
+      <c r="F2" s="4" t="n">
         <v>44805</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="L2" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="C3" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D3" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="E3" s="4" t="n">
+      <c r="E3" s="3" t="n">
         <v>44722</v>
       </c>
-      <c r="F3" s="5" t="n">
+      <c r="F3" s="4" t="n">
         <v>44810</v>
       </c>
       <c r="G3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="K3" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="L3" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="N3" s="6" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="E4" s="4" t="n">
+      <c r="E4" s="3" t="n">
         <v>44905</v>
       </c>
-      <c r="F4" s="5" t="n">
+      <c r="F4" s="4" t="n">
         <v>44816</v>
       </c>
       <c r="G4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J4" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="K4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="3" t="n">
+        <v>44905</v>
+      </c>
+      <c r="F5" s="4" t="n">
+        <v>44816</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="L4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="N4" s="6" t="s">
-        <v>21</v>
+      <c r="J5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="7" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E7" s="5"/>
+      <c r="E7" s="4"/>
     </row>
     <row r="8" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E8" s="5"/>
+      <c r="E8" s="4"/>
     </row>
     <row r="9" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E9" s="5"/>
+      <c r="E9" s="4"/>
     </row>
   </sheetData>
   <dataValidations count="3">
@@ -1122,7 +1120,7 @@
       <c r="C2" s="1" t="n">
         <v>80</v>
       </c>
-      <c r="D2" s="4" t="n">
+      <c r="D2" s="3" t="n">
         <v>44571</v>
       </c>
     </row>
@@ -1136,7 +1134,7 @@
       <c r="C3" s="1" t="n">
         <v>81</v>
       </c>
-      <c r="D3" s="4" t="n">
+      <c r="D3" s="3" t="n">
         <v>44722</v>
       </c>
     </row>
@@ -1150,7 +1148,7 @@
       <c r="C4" s="1" t="n">
         <v>82</v>
       </c>
-      <c r="D4" s="4" t="n">
+      <c r="D4" s="3" t="n">
         <v>44905</v>
       </c>
     </row>

</xml_diff>